<commit_message>
PubMed Calls Code Refactoring
</commit_message>
<xml_diff>
--- a/Excel_Files/PubMed_Central_Searches.xlsx
+++ b/Excel_Files/PubMed_Central_Searches.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jogeo\Desktop\Project\Blood-Brain-Barrier-Drug-Prediction\Excel_Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A2B6F4D-1C06-4482-9160-C5B19D3087AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26AF54AE-A589-4228-B457-99C2E22639D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3273,7 +3273,7 @@
   <dimension ref="A1:J362"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3711,7 +3711,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>8116309</v>
       </c>
@@ -3731,7 +3731,7 @@
         <v>368</v>
       </c>
       <c r="G15" t="s">
-        <v>705</v>
+        <v>707</v>
       </c>
       <c r="H15" t="s">
         <v>708</v>

</xml_diff>